<commit_message>
importação de perguntas integrar servidor de homolagação
</commit_message>
<xml_diff>
--- a/excel/perguntas_e_respostas_procon_04_05.xlsx
+++ b/excel/perguntas_e_respostas_procon_04_05.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="329">
   <si>
     <t>Categoria</t>
   </si>
@@ -36,8 +36,7 @@
   </si>
   <si>
     <t>Os alimentos possuem determinadas características fundamentais, descritas nas informações constantes nas suas embalagens. Alimentos estragados (impróprios para o consumo), deteriorados (qualidade inferior à prevista), corrompidos (embalagens rompidas, abertas) ou contaminados (que tenham em sua composição ou apresentação elementos ou objetos inesperados) perderam essas qualidades.
-É direito do consumidor exigir a troca do alimento ao comerciante (vendedor direto, mercados, supermercados) ou ao fornecedor (vendedor indireto) ou a devolução do dinheiro.
-</t>
+É direito do consumidor exigir a troca do alimento ao comerciante (vendedor direto, mercados, supermercados) ou ao fornecedor (vendedor indireto) ou a devolução do dinheiro.</t>
   </si>
   <si>
     <t>4.1.2. O que devo fazer em caso de intoxicação alimentar?</t>
@@ -53,8 +52,7 @@
 De acordo com o art. 6º, inciso III, da Lei federal nº 8.078/90, os produtos devem conter as seguintes informações adequadas e claras: especificações corretas de quantidade, características, composição, qualidade, tributos incidentes e preço, bem como sobre os riscos que apresentem.
 Por sua vez,  se o consumidor for uma pessoa com deficiência, as informações deverão ser acessíveis, 
 Além disso, a composição de alguns alimentos pode causar problemas de saúde aos consumidores que possuam intolerância, como por exemplo alimentos que contém glúten.
-Segundo a Lei federal nº 10.674/03, todos os alimentos industrializados deverão conter em seu rótulo e bula, obrigatoriamente, as inscrições "contém Glúten" ou "não contém Glúten", conforme o caso. A advertência deve ser impressa nos rótulos e embalagens dos produtos respectivos assim como em cartazes e materiais de divulgação em caracteres com destaque, nítidos e de fácil leitura.
-</t>
+Segundo a Lei federal nº 10.674/03, todos os alimentos industrializados deverão conter em seu rótulo e bula, obrigatoriamente, as inscrições "contém Glúten" ou "não contém Glúten", conforme o caso. A advertência deve ser impressa nos rótulos e embalagens dos produtos respectivos assim como em cartazes e materiais de divulgação em caracteres com destaque, nítidos e de fácil leitura.</t>
   </si>
   <si>
     <t>4.1.4. Onde posso me informar sobre características e regulamentos abrangentes dos alimentos industrializados, inclusive informações em embalagens ou rótulos ?</t>
@@ -77,8 +75,7 @@
   <si>
     <t>Em regra, bancos e instituições financeiras se sujeitam ao Código de Defesa do Consumidor, inclusive no que se refere a serviços securitários e fundos de investimento. O mesmo vale para cooperativas de crédito, que também integram o sistema financeiro nacional. Assim, na maioria dos contratos envolvendo pessoas físicas, os contratos bancários são relações de consumo, como é o caso da conta corrente. 
 No entanto, algumas vezes, a finalidade da relação bancária é fomentar o negócio do contratante, como por exemplo, a contratação de empréstimo para fomento da empresa. Nesses casos, não haverá relação de consumo. 
-Portanto, a característica que definirá se o contrato bancário é uma relação de consumo é a parte ser destinatária final dos produtos ou serviços contratados.
-</t>
+Portanto, a característica que definirá se o contrato bancário é uma relação de consumo é a parte ser destinatária final dos produtos ou serviços contratados.</t>
   </si>
   <si>
     <t>4.2.2. Quem representa o consumidor perante o Banco Central do Brasil? Como se dá a participação na formulação das normas?</t>
@@ -94,12 +91,11 @@
 Assim, os produtos e serviços considerados essenciais (prioritários) não podem ser “tarifados” nos termos da Resolução nº 3.919/10, do Conselho Monetário Nacional. http://www.bcb.gov.br/pre/normativos/busca/downloadNormativo.asp?arquivo=/Lists/Normativos/Attachments/49514/Res_3919_v4_P.pdf</t>
   </si>
   <si>
-    <t>4.2.4. O que fazer se os juros cobrados pelas instituições financeiras forem abusivos ? </t>
+    <t>4.2.4. O que fazer se os juros cobrados pelas instituições financeiras forem abusivos ?</t>
   </si>
   <si>
     <t>Se os juros forem abusivos, além da devolução da quantia cobrada, são cabíveis o ressarcimento por danos materiais e morais eventualmente observados. É o caso da inviabilidade do crédito por inscrição do nome do consumidor nos cadastros de proteção ao crédito.
-Em qualquer caso, cabe também a revisão da cláusula que prevê juros abusivos.
-</t>
+Em qualquer caso, cabe também a revisão da cláusula que prevê juros abusivos.</t>
   </si>
   <si>
     <t>4.2.5. Se a instituição financeira for liquidada, quem responde pelos danos causados ao consumidor?</t>
@@ -139,8 +135,7 @@
   </si>
   <si>
     <t>A Lei federal nº 8.078/90 – Código de Defesa do Consumidor continua sendo a previsão legislativa fundamental dos direitos do consumidor.
-No entanto, devido às peculiaridades do comércio eletrônico, foi editado o Decreto federal nº 7.962/13, que trouxe obrigações aos fornecedores sobre a) forma de prestação de informações claras a respeito do produto, serviço e do próprio fornecedor;b) o modo de atendimento facilitado ao ; e c) como possibilitar o direito de arrependimento.
-</t>
+No entanto, devido às peculiaridades do comércio eletrônico, foi editado o Decreto federal nº 7.962/13, que trouxe obrigações aos fornecedores sobre a) forma de prestação de informações claras a respeito do produto, serviço e do próprio fornecedor;b) o modo de atendimento facilitado ao ; e c) como possibilitar o direito de arrependimento.</t>
   </si>
   <si>
     <t>4.6.2. Os sites de vendas coletivas também são responsáveis pelos problemas com produtos e serviços?</t>
@@ -155,24 +150,21 @@
     <t>O dever de cancelar a ordem de pagamento é do fornecedor.
 O direito de arrependimento prevê que consumidor pode desistir do contrato, no prazo de 7 dias a contar de sua assinatura ou do ato de recebimento do produto ou serviço, sempre que a contratação de fornecimento de produtos e serviços ocorrer fora do estabelecimento comercial, especialmente por telefone ou a domicílio.
 Se o consumidor exercitar o direito de arrependimento, os valores eventualmente pagos, a qualquer título, durante o prazo de reflexão, serão devolvidos, de imediato, monetariamente atualizados.
-Assim, comunicado do arrependimento, o fornecedor deverá responder imediatamente ao consumidor e informar ao banco ou administradora do cartão para não lançar a transação ou estornar os valores lançados.
-</t>
+Assim, comunicado do arrependimento, o fornecedor deverá responder imediatamente ao consumidor e informar ao banco ou administradora do cartão para não lançar a transação ou estornar os valores lançados.</t>
   </si>
   <si>
     <t>4.6.4. Se o fornecedor ou comerciante não informar ao banco ou à administradora sobre o cancelamento da compra, como devo agir?</t>
   </si>
   <si>
     <t>Constatada a irregularidade, o consumidor deverá procurar o PROCON para tentar resolver a situação através de comunicação oficial ou acordo.
-Além disso, o PROCON orientará sobre as medidas que poderão ser adotadas no caso de danos (prejuízos) emergentes.
-</t>
+Além disso, o PROCON orientará sobre as medidas que poderão ser adotadas no caso de danos (prejuízos) emergentes.</t>
   </si>
   <si>
     <t>4.6.5. Exercido o direito de arrependimento, mas recebido o produto na residência, como deve ser efetuada a devolução?</t>
   </si>
   <si>
     <t>Se o produto recebido for de pequeno porte, a devolução poderá ser feita pelo mesmo modo com que foi recebida, geralmente utilizando-se de serviços de entrega.
-Se o produto recebido for de grande porte, o fornecedor ou comerciante deverá retirá-lo gratuitamente, pois a mera incomodidade faz parte do risco do negócio.
-</t>
+Se o produto recebido for de grande porte, o fornecedor ou comerciante deverá retirá-lo gratuitamente, pois a mera incomodidade faz parte do risco do negócio.</t>
   </si>
   <si>
     <t>4.6.6. Como os contratos devem ser apresentados pelo fornecedor no site?</t>
@@ -193,8 +185,7 @@
 c) com idade entre 15 e 29 anos e comprovadamente carente (Lei federal nº 12.933/13);
 d) que possuam deficiência física (Lei federal nº 12.933/13 e Lei Municipal 12975/00); ou
 e) acompanhantes de deficiente físico durante o evento (Lei federal nº 12.933/13).
-Além dessas, há regras específicas editadas pelos Estados e Municípios que também podem conceder o benefício.
-</t>
+Além dessas, há regras específicas editadas pelos Estados e Municípios que também podem conceder o benefício.</t>
   </si>
   <si>
     <t>4.7.2. Como deverá agir o consumidor se seu direito à meia-entrada não for atendido pelos estabelecimento?</t>
@@ -202,8 +193,7 @@
   <si>
     <t>O consumidor poderá adquirir o ingresso pelo valor integral e requerer, após o espetáculo, a devolução do que pagou.
 Caso não receba a devolução, poderá acionar o PROCON para tentar resolver o conflito.
-Se a iniciativa administrativa não resolver a questão, deverá recorrer ao Poder Judiciário.
-</t>
+Se a iniciativa administrativa não resolver a questão, deverá recorrer ao Poder Judiciário.</t>
   </si>
   <si>
     <t>4.7.3. Quais são os benefícios da meia-entrada concedidos no âmbito do Município de São Paulo ?</t>
@@ -213,8 +203,7 @@
 Além daqueles referidos no item 4.7.1, têm direito àmeia entrada:
 a) Diretores, coordenadores pedagógicos, supervisores e membros do quadro de apoio das escolas das redes estadual e municipais, mediante apresentaçãode carteira funcional ou holerite e RG (Lei estadual nº 15.289/2014);
 b) professores da rede pública estadual e das redes municipais de ensino, exercendo docência nos níveis infantil, fundamental e médio, mediante apresentação de carteira funcional ou holerite e RG (Lei Estadual 14729/2012;
-c) estudantes que residam no município de São Paulo e que estejam matriculados em cursos profissionalizantes (básico e técnico), pré-vestibulares e pós-graduação (Lei Municipal nº 13.71/2004).
-</t>
+c) estudantes que residam no município de São Paulo e que estejam matriculados em cursos profissionalizantes (básico e técnico), pré-vestibulares e pós-graduação (Lei Municipal nº 13.71/2004).</t>
   </si>
   <si>
     <t>Educacao**</t>
@@ -239,15 +228,14 @@
   </si>
   <si>
     <t>Não, conforme dispõe o art. 5º, da Lei federal nº 9.870/99.
-No entanto, não poderá ocorrer constrangimento ou retenção/sonegação de documentos por parte do estabelecimento.
-</t>
+No entanto, não poderá ocorrer constrangimento ou retenção/sonegação de documentos por parte do estabelecimento.</t>
   </si>
   <si>
     <t>4.8.1.4. A instituição de ensino poderá reajustar as mensalidades após a fixação inicial prevista em contrato?</t>
   </si>
   <si>
     <r>
-      <t>Não. As mensalidades somente poderão ser reajustadas um ano após sua fixação. </t>
+      <t>Não. As mensalidades somente poderão ser reajustadas um ano após sua fixação.</t>
     </r>
     <r>
       <rPr>
@@ -286,8 +274,7 @@
 b) A operadora comprova que a interrupção do serviço foi causada pelo próprio consumidor;.
 c) A interrupção do serviçofoi causada para manutenção preventiva ou ampliações da rede e não excedeu o total de 24 horas no mês de referência. No entanto, para caracterizar tal hipótese, a interrupção e seu tempo de duração devem ser informados ao consumidor pela operadora com a antecedência mínima de 3 dias. Caso não haja a informação prévia da interrupção ao consumidor ou o tempo de interrupção exceda o limite mensal de 24 horas, o consumidor tem direito ao abatimento/ressarcimento. Fundamentação Legal: 
 - Artigo 20 da Lei nº 8.078/90 e Resolução nº 488/2007 da Anatel
-Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.
-</t>
+Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.</t>
   </si>
   <si>
     <t>2. Atrasei o pagamento da minha conta de TV por assinatura. Quais são os encargos devidos pelo atraso no pagamento ?</t>
@@ -297,8 +284,7 @@
  - Multa não superior a 2% ao mês;
  - Correção monetária e juros de mora não superiores a 1% ao mês. Fundamentação legal:
 - Artigo 100, parágrafo único, da Resolução nº 632/2014 da ANATEL
-Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.
-</t>
+Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.</t>
   </si>
   <si>
     <t>3. Estou inadimplente com o pagamento da minha TV por assinatura. A empresa pode suspender a prestação do serviço ?</t>
@@ -336,7 +322,7 @@
 Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.</t>
   </si>
   <si>
-    <t>6. Quais são as regras aplicáveis ao cancelamento do serviço de TV por assinatura </t>
+    <t>6. Quais são as regras aplicáveis ao cancelamento do serviço de TV por assinatura</t>
   </si>
   <si>
     <t>O cancelamento do serviço independe do pagamento de eventuais débitos em nome do consumidor. No ato de cancelamento, deve ser assegurado o direito à informação sobre eventuais condições aplicáveis à rescisão e multas incidentes por descumprimento de prazos contratuais de permanência mínima.
@@ -354,8 +340,7 @@
     <t>O prazo máximo é de 48 horas, contadas da solicitação do consumidor.
 Fundamentação Legal: 
 Resolução nº 411/2005 da Anatel.
-Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.
-</t>
+Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.</t>
   </si>
   <si>
     <t>8. O meu plano de serviço de TV por assinatura pode ser alterado sem aviso prévio?</t>
@@ -366,8 +351,7 @@
 Caso a alteração implique na retirada de algum canal do plano contratado, a empresa deve substituí-lo por outro do mesmo gênero ou realizar desconto na mensalidade paga, sempre a critério do consumidor.
 Fundamentação Legal: 
 - Artigo 52 da Resolução nº 632/2014 da Anatel e artigo 28 da Resolução nº 488/2007 da Anatel.
-Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.
-</t>
+Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.</t>
   </si>
   <si>
     <t>9. O que é contrato de permanência ou fidelização ?</t>
@@ -379,8 +363,7 @@
 Não é devida a multa se o cancelamento do serviço for solicitado em virtude de descumprimento de obrigação contratual ou legal da prestadora de serviço de TV por assinatura.
 Fundamentação Legal: 
 Arts. 57 a 59 da Resolução nº 632/2014.
-Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.
-</t>
+Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.</t>
   </si>
   <si>
     <t>10. A empresa de TV por assinatura pode cobrar pela instalação e pela programação de ponto-extra ?</t>
@@ -389,8 +372,7 @@
     <t>A empresa pode cobrar pela instalação de pontos-extras. No entanto, o consumidor deve pagar apenas pela programação do ponto-principal. Não pode ser cobrado valor adicional pela programação transmitida nos pontos-extras instalados no mesmo endereço residencial do consumidor, inclusive na hipótese de pay-per-view. 
 Fundamentação Legal: 
 Artigos 29 e 30 da Resolução nº 488/2007 da Anatel
-Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.
-</t>
+Para maiores informações, CLIQUE AQUI para acessar o sítio eletrônico da ANATEL.</t>
   </si>
   <si>
     <t>Telemarketing e Serviços de Atendimento ao Cliente (SAC)</t>
@@ -406,8 +388,7 @@
   </si>
   <si>
     <t>Nem todo serviço de atendimento ao consumidor possui regulamentação. 
-O Decreto nº 6.523/08, conhecido como a Lei do SAC, que regulamenta os serviços de atendimento ao consumidor, é aplicável apenas aos fornecedores de serviços regulados pelo Poder Público federal, tais como telefonia, energia elétrica, TV por assinatura, planos de saúde, aviação, transporte terrestre, seguradoras, instituições financeiras, etc. Todavia, não são aplicáveis as regras constantes do Decreto nº 6.523/08 à oferta e a contratação de produtos e serviços realizadas por telefone por estas empresas.
-</t>
+O Decreto nº 6.523/08, conhecido como a Lei do SAC, que regulamenta os serviços de atendimento ao consumidor, é aplicável apenas aos fornecedores de serviços regulados pelo Poder Público federal, tais como telefonia, energia elétrica, TV por assinatura, planos de saúde, aviação, transporte terrestre, seguradoras, instituições financeiras, etc. Todavia, não são aplicáveis as regras constantes do Decreto nº 6.523/08 à oferta e a contratação de produtos e serviços realizadas por telefone por estas empresas.</t>
   </si>
   <si>
     <t>3. Quais são os principais direitos assegurados pelo Decreto nº 6.523/08, conhecido como Lei do SAC?</t>
@@ -423,8 +404,7 @@
 • É proibido solicitar a repetição da demanda do consumidor após seu registro pelo primeiro atendente;
 • O SAC garantirá a transferência imediata ao setor competente para atendimento definitivo da demanda do consumidor. Caso o primeiro atendente não tenha essa atribuição, a transferência da ligação para o setor competente deve ser efetivada em até sessenta segundos;
 • Nos casos de reclamação e cancelamento de serviço, não será admitida a transferência da ligação, devendo todos os atendentes possuir atribuições para executar essas funções;
-• É proibida a veiculação de mensagens publicitárias durante o tempo de espera para o atendimento, salvo se houver prévio consentimento do consumidor;
-</t>
+• É proibida a veiculação de mensagens publicitárias durante o tempo de espera para o atendimento, salvo se houver prévio consentimento do consumidor;</t>
   </si>
   <si>
     <t>• O SAC garantirá a transferência imediata ao setor competente para atendimento definitivo da demanda do consumidor. Caso o primeiro atendente não tenha essa atribuição, a transferência da ligação para o setor competente deve ser efetivada em até sessenta segundos;
@@ -432,14 +412,11 @@
 • É proibida a veiculação de mensagens publicitárias durante o tempo de espera para o atendimento, salvo se houver prévio consentimento do consumidor;
 • As informações solicitadas pelos consumidores deverão ser imediatamente atendidas e as pendências resolvidas no prazo máximo de 05 dias úteis;
 • O consumidor será informado sobre a resolução de sua demanda e, sempre que solicitar, deve ser enviada a comprovação pertinente por correspondência ou por meio eletrônico, a seu critério;. 
-• A resposta do fornecedor, além de clara e objetiva, deve abordar todos os pontos da demanda do consumidor;. 
-</t>
-  </si>
-  <si>
-    <t>
-• Quando a demanda do consumidor versar sobreou cobrança indevida ou serviço não solicitado, a cobrança deve ser suspensa imediatamente, salvo se o fornecedor indicar o instrumento por meio do qual o serviço foi contratado e comprovar que o valor é efetivamente devido;.
-• O SAC deve receber e processar imediatamente o pedido de cancelamento de serviço feito pelo consumidor. Os efeitos do cancelamento são imediatos à solicitação, ainda que o seu processamento técnico necessite de prazo e haja débitos do consumidor em aberto. O comprovante do pedido de cancelamento deve ser expedido por correspondência ou por meio eletrônico, a critério do consumidor. 
-</t>
+• A resposta do fornecedor, além de clara e objetiva, deve abordar todos os pontos da demanda do consumidor;.</t>
+  </si>
+  <si>
+    <t>• Quando a demanda do consumidor versar sobreou cobrança indevida ou serviço não solicitado, a cobrança deve ser suspensa imediatamente, salvo se o fornecedor indicar o instrumento por meio do qual o serviço foi contratado e comprovar que o valor é efetivamente devido;.
+• O SAC deve receber e processar imediatamente o pedido de cancelamento de serviço feito pelo consumidor. Os efeitos do cancelamento são imediatos à solicitação, ainda que o seu processamento técnico necessite de prazo e haja débitos do consumidor em aberto. O comprovante do pedido de cancelamento deve ser expedido por correspondência ou por meio eletrônico, a critério do consumidor.</t>
   </si>
   <si>
     <t>4. Existe um tempo máximo para o contato direto do consumidor com o atendente do SAC, quando essa opção for selecionada ?</t>
@@ -449,8 +426,7 @@
 • Em regra, o tempo máximo para o  contato direto  com o  atendente é de 60 segundos;
 • Nos serviços financeiros, o tempo máximo para o contato direto  com o  atendente é de 45 segundos.  Nas segundas-feiras, nos  dias  que  antecedem e  sucedem  os feriados e no 5º dia útil de cada mês, o prazo máximo é de 90 segundos;.
 • Nos serviços de energia elétrica, o tempo máximo para ocontato  direto  com  o  atendente é de 60 segundos, ressalvados os casos  de  atendimentos emergenciais  de abrangência  sistêmica, assim  considerados aqueles  que,  por sua  própria  natureza, impliquem  a interrupção  do  fornecimento de  energia elétrica  a um  grande número  de  consumidores, ocasionando  elevadaconcentração de chamadas.
-Os prazos máximos fixados na Portaria nº 2.014/08 não excluem outros mais benéficos ao consumidor, decorrentes de regulamentações e contratos de concessão.
-</t>
+Os prazos máximos fixados na Portaria nº 2.014/08 não excluem outros mais benéficos ao consumidor, decorrentes de regulamentações e contratos de concessão.</t>
   </si>
   <si>
     <t>5. Por quanto tempo as gravações do atendimento devem ser armazenadas pelo SAC ? Qual o prazo máximo para a entrega da gravação do atendimento ao consumidor ? Há alguma sanção para a empresa que recusa ou dificulta a entrega ?</t>
@@ -459,8 +435,7 @@
     <t>O Decreto nº 6.523/08 estipula que as empresas prestadoras de serviços regulados pelo Poder Público federal devem gravar as conversas mantidas pelos seus serviços de atendimento ao consumidor e armazená-las pelo prazo mínimo de 90 dias, durante o qual o consumidor poderá requerer acesso ao seu conteúdo.
 De acordo com a Portaria nº 29/09, editada pelo Ministério da Justiça, o prazo máximo para a entrega da gravação do atendimento realizado pelo SAC é de 10 dias. A entrega pode ser realizada eletronicamente, por correspondência ou pessoalmente, sendo facultada a escolha ao consumidor.
 Recusar ou dificultar a entrega da gravação do atendimento realizado pelo SAC constitui prática abusiva e sujeita o fornecedor às sanções previstas na Lei nº 8.078/90. 
-A recusa da entrega da gravação também  faz presumir a veracidade da reclamação do consumidor quanto à violação do Decreto nº 6.523/08. A referida presunção é relativa, ou seja, admite prova em contrário a ser produzida pelo fornecedor.
-</t>
+A recusa da entrega da gravação também  faz presumir a veracidade da reclamação do consumidor quanto à violação do Decreto nº 6.523/08. A referida presunção é relativa, ou seja, admite prova em contrário a ser produzida pelo fornecedor.</t>
   </si>
   <si>
     <t>Transporte rodoviario</t>
@@ -471,22 +446,20 @@
   <si>
     <t>O DPVAT é um seguro de trânsito pago obrigatoriamente pelas empresas de ônibus para cobrir os danos pessoais causados pelos veículos automotores de via terrestre. O pagamento deste seguro pela empresa de transporte já confere ao passageiro o pagamento de indenizações em caso de morte ou invalidez, bem como reembolso, em caso de despesas médicas em decorrência de acidentes. Os valores das indenizações, definidos em lei, são fixos.
 Por sua vez, o seguro complementar de viagem é um contrato de seguro geralmente comercializado pelas empresas de transporte rodoviário no ato de venda da passagem com o fim de complementar o valor da indenização/reembolso do DPVAT ou garantir uma cobertura maior àquelaoferecida pelo DPVAT.
-Tanto as Resoluções nº 1.454/06 e 4.282/14, ambas da ANTT, relativas ao transporte rodoviário interestadual e internacional de passageiros, quanto o Decreto Estadual nº 29.913/89, que regulamenta o transporte intermunicipal de passageiros no Estado de São Paulo, estabelecem que a contratação do seguro complementar de viagem é facultativa e seu preço não pode estar vinculado ao valor da passagem. O consumidor não é obrigado a contratá-lo.
-</t>
+Tanto as Resoluções nº 1.454/06 e 4.282/14, ambas da ANTT, relativas ao transporte rodoviário interestadual e internacional de passageiros, quanto o Decreto Estadual nº 29.913/89, que regulamenta o transporte intermunicipal de passageiros no Estado de São Paulo, estabelecem que a contratação do seguro complementar de viagem é facultativa e seu preço não pode estar vinculado ao valor da passagem. O consumidor não é obrigado a contratá-lo.</t>
   </si>
   <si>
     <t>2. Qual a validade do bilhete de passagem de transporte rodoviário intermunicipal, interestadual e internacional ?</t>
   </si>
   <si>
-    <t>De acordo com a Lei nº 11.975/09, os bilhetes de passagens adquiridos no transporte coletivo rodoviário de passageiros intermunicipal, interestadual e internacional possuem validade de um ano, a partir da data de sua emissão, independentemente de estarem com data e horários marcados. </t>
+    <t>De acordo com a Lei nº 11.975/09, os bilhetes de passagens adquiridos no transporte coletivo rodoviário de passageiros intermunicipal, interestadual e internacional possuem validade de um ano, a partir da data de sua emissão, independentemente de estarem com data e horários marcados.</t>
   </si>
   <si>
     <t>3. Comprei uma passagem de transporte rodoviário interestadual/ internacional, mas desisti de viajar. Tenho direito ao reembolso do valor pago ?</t>
   </si>
   <si>
     <t>De acordo com a Resolução nº 4.282/14da ANTT, o passageiro possui direito ao reembolso se desistir da viagem até 3 horas antes do horário do embarque constante do bilhete, hipótese em que a empresa de transporte poderá reter até 5% do valor da passagem, a título de comissão de venda e multa compensatória.
-Não há direito a reembolso, se o passageiro não comparecer para embarque ou não manifestar sua vontade de desistir da viagem até 3 horas antes do horário do embarque constante do bilhete, porém fica mantida a validade da passagem para remarcação e/ou transferência por até um ano, a partir da data de sua primeira emissão.
-</t>
+Não há direito a reembolso, se o passageiro não comparecer para embarque ou não manifestar sua vontade de desistir da viagem até 3 horas antes do horário do embarque constante do bilhete, porém fica mantida a validade da passagem para remarcação e/ou transferência por até um ano, a partir da data de sua primeira emissão.</t>
   </si>
   <si>
     <t>4. Preciso remarcarum bilhete de passagem de transporte rodoviário interestadual/ internacional. A empresa pode cobrar taxa ?</t>
@@ -502,8 +475,7 @@
 1. Continuar a viagem em outra empresa às expensas da transportadora responsável pelo atraso; 
 2. Receber de imediato o valor do bilhete de passagem, em caso de desistência; 
 3. Continuar a viagem pela mesma transportadora, que deverá dar continuidade à viagem num período máximo de 3 (três) horas após a interrupção.
-Caso o atraso seja superior a 3 horas e a empresa for por ele responsável, a alimentação e eventual hospedagem do passageiro correrão às expensas da transportadora.
-</t>
+Caso o atraso seja superior a 3 horas e a empresa for por ele responsável, a alimentação e eventual hospedagem do passageiro correrão às expensas da transportadora.</t>
   </si>
   <si>
     <t>Transporte Aereo</t>
@@ -534,8 +506,7 @@
 Além da assistência material, em caso de espera superior a 4 horas em aeroporto de escala ou de conexão ,o consumidor pode optar:
  - Pela reacomodação em voo próprio ou de terceiro, que ofereça serviço equivalente para o mesmo destino, na primeira oportunidade; 
  - Pelo reembolso integral, assegurado o retorno ao aeroporto de origem; ou do trecho não utilizado, se o deslocamento já realizado aproveitar ao passageiro;
- - A conclusão do serviço por outra modalidade de transporte.
-</t>
+ - A conclusão do serviço por outra modalidade de transporte.</t>
   </si>
   <si>
     <t>4. Minha bagagem foi extraviada.  O que devo fazer ?</t>
@@ -562,8 +533,7 @@
     <t>2. O que é prêmio do seguro? Se eu atrasar o pagamento do prêmio, a seguradora deve cobrir eventual sinistro ?</t>
   </si>
   <si>
-    <t>Prêmio de seguro é o valor pago pela contratação do seguro. O atraso do pagamento do prêmio pode implicar na suspensão ou até mesmo o cancelamento do seguro, prejudicando o direito à indenização, caso o sinistro ocorra após a data de suspensão ou cancelamento. O contrato deverá conter cláusula informando as hipóteses em que ocorre a suspensão e/ou o cancelamento do contrato de seguro em razão da falta de pagamento de prêmio.
-</t>
+    <t>Prêmio de seguro é o valor pago pela contratação do seguro. O atraso do pagamento do prêmio pode implicar na suspensão ou até mesmo o cancelamento do seguro, prejudicando o direito à indenização, caso o sinistro ocorra após a data de suspensão ou cancelamento. O contrato deverá conter cláusula informando as hipóteses em que ocorre a suspensão e/ou o cancelamento do contrato de seguro em razão da falta de pagamento de prêmio.</t>
   </si>
   <si>
     <t>3. O que se entende por perda de direito?</t>
@@ -574,24 +544,21 @@
  - o sinistro ocorre por culpa grave ou dolo do segurado ou beneficiário do seguro;
  - a reclamação de indenização por sinistro for fraudulenta ou de má-fé;
  - o segurado, corretor, beneficiários ou ainda seus representantes e prepostos fizerem declarações falsas ou, por qualquer meio, tentarem obter benefícios ilícitos do seguro;
- - o segurado agravar intencionalmente o risco.
-</t>
+ - o segurado agravar intencionalmente o risco.</t>
   </si>
   <si>
     <t>4. A seguradora poderá recusar uma proposta de seguro?</t>
   </si>
   <si>
     <t>Sim, porém a seguradora deve comunicar ao consumidor a não aceitação do seguro e justificar a recusa.
-A seguradora tem o prazo de 15 dias para se manifestar quanto à proposta de seguro, seja para seguros novos ou renovações, bem como para alterações que impliquem na modificação do risco. Findo o prazo, sem que haja recusa pela seguradora, o seguro passa a ser considerado aceito.
-</t>
+A seguradora tem o prazo de 15 dias para se manifestar quanto à proposta de seguro, seja para seguros novos ou renovações, bem como para alterações que impliquem na modificação do risco. Findo o prazo, sem que haja recusa pela seguradora, o seguro passa a ser considerado aceito.</t>
   </si>
   <si>
     <t>5. Qual o prazo para receber a indenização da seguradora?</t>
   </si>
   <si>
     <t>O prazo máximo é de 30 dias, contados da entrega de todos os documentos básicos apresentados pelo segurado ou beneficiários. Esse prazo pode ser suspenso quando, de forma justificada, forem solicitados novos documentos.
-Em caso de sinistro, é importante que o consumidor solicite à seguradora o protocolo que identifique a data do recebimento do aviso de sinistro e respectivos documentos.
-</t>
+Em caso de sinistro, é importante que o consumidor solicite à seguradora o protocolo que identifique a data do recebimento do aviso de sinistro e respectivos documentos.</t>
   </si>
   <si>
     <t>6. A garantia estendida é uma espécie de seguro ? Quais são as coberturas oferecidas?</t>
@@ -601,8 +568,7 @@
 O seguro de Garantia Estendida pode oferecer uma das seguintes coberturas básicas:
 a) Extensão de garantia original: contrato cuja vigência inicia-se após o término da garantia do fornecedor e que contempla as mesmas coberturas e exclusões oferecidas pela garantia do fornecedor;
 b) Extensão de garantia original ampliada: contrato cuja vigência inicia-se após o término da garantia do fornecedor e que contempla as mesmas coberturas oferecidas pela garantia do fornecedor, apresentando, adicionalmente, a inclusão de novas coberturas, desde que não enquadradas em outros ramos específicos de seguro;
-c) Extensão de garantia reduzida: contrato cuja vigência inicia-se após o término da garantia do fornecedor e que pode contemplar coberturas reduzidas comparativamente àquelas oferecidas pela garantia do fornecedor. Esta modalidade aplica-se somente a veículos automotores e a bens que possuem apenas garantia legal.
-</t>
+c) Extensão de garantia reduzida: contrato cuja vigência inicia-se após o término da garantia do fornecedor e que pode contemplar coberturas reduzidas comparativamente àquelas oferecidas pela garantia do fornecedor. Esta modalidade aplica-se somente a veículos automotores e a bens que possuem apenas garantia legal.</t>
   </si>
   <si>
     <t>Recall</t>
@@ -625,16 +591,14 @@
   <si>
     <t>Para saber se há recall para determinado produto, o consumidor deve entrar em contato direto com o fornecedor.
 Alternativamente, pode ser consultado o sistema online de recalls do Departamento de Proteção e Defesa do Consumidor, no link http://portal.mj.gov.br/recall.
-Desde o ano de 2011, o Departamento Nacional de Trânsito possui sistema de consulta para verificar se determinado veículo é objeto de recall. Para acessar o referido sistema, CLIQUE AQUI  (https://denatran.serpro.gov.br ). As campanhas de recall não atendidas em um ano pelo consumidor passam a constar do documento do veículo.
-</t>
+Desde o ano de 2011, o Departamento Nacional de Trânsito possui sistema de consulta para verificar se determinado veículo é objeto de recall. Para acessar o referido sistema, CLIQUE AQUI  (https://denatran.serpro.gov.br ). As campanhas de recall não atendidas em um ano pelo consumidor passam a constar do documento do veículo.</t>
   </si>
   <si>
     <t>4. Há prazo para o consumidor atender ao recall?</t>
   </si>
   <si>
     <t>Não. O recall só é finalizado quando o risco à saúde e segurança for eliminado do mercado de consumo, ou seja, quando todos os produtos afetados pelo defeito forem reparados ou recolhidos pelo fornecedor.
-Embora seja comum a divulgação de um prazo para o recall, o fornecedor é obrigado a reparar o problema a qualquer momento e sem qualquer custo ao consumidor.
-</t>
+Embora seja comum a divulgação de um prazo para o recall, o fornecedor é obrigado a reparar o problema a qualquer momento e sem qualquer custo ao consumidor.</t>
   </si>
   <si>
     <t>5. O não atendimento ao recall pelo consumidor exclui a responsabilidade do fornecedor por eventual dano?</t>
@@ -661,7 +625,7 @@
     <t>3. No meu ticket de estacionamento consta que o estacionamento não se responsabiliza por danos ao veículo, nem por objetos deixados em seu interior. Esse aviso tem valor legal?</t>
   </si>
   <si>
-    <t>Não. Tais avisos configuram verdadeiras cláusulas de não-indenizar e, de acordo com os artigos 25 e 51 do Código de Defesa do Consumidor, são consideradas abusivas e não possuem qualquer validade. Os estacionamentos assumem a obrigação de guarda e vigilância dos veículos e respondem pela reparação dos danos causados aos consumidores pela prestação dos seus serviços, de acordo com o artigo 14 do Código de Defesa do Consumidor. </t>
+    <t>Não. Tais avisos configuram verdadeiras cláusulas de não-indenizar e, de acordo com os artigos 25 e 51 do Código de Defesa do Consumidor, são consideradas abusivas e não possuem qualquer validade. Os estacionamentos assumem a obrigação de guarda e vigilância dos veículos e respondem pela reparação dos danos causados aos consumidores pela prestação dos seus serviços, de acordo com o artigo 14 do Código de Defesa do Consumidor.</t>
   </si>
   <si>
     <t>4. Os serviços de “valet service” podem parar meu veículo em via pública ? Essas empresas devem possuir seguro? Ao receber meu carro, essas empresas podem inspecioná-lo?</t>
@@ -669,8 +633,7 @@
   <si>
     <t>De acordo com a Lei Municipal nº 13.763/04, na prestação dos serviços de “valet” é proibido o uso de via pública para o estacionamento de veículos.  Inclusive, esses serviços devem afixar em local visível o endereço onde os veículos são estacionados.
 A referida lei ainda estabelece a obrigatoriedade dessas empresas possuírem seguro com cobertura de incêndio, furto, roubo, colisão e quaisquer danos materiais causados ao veículo, bem como seguro de percurso.
-Os “valets” podem inspecionar o veículo quando de sua entrega. Nesse momento, a empresa deve emitir recibo a ser entregue ao consumidor com anotação do modelo, marca, placa e quilometragem do automóvel, bem como da existência de eventual avaria nele existente. 
-</t>
+Os “valets” podem inspecionar o veículo quando de sua entrega. Nesse momento, a empresa deve emitir recibo a ser entregue ao consumidor com anotação do modelo, marca, placa e quilometragem do automóvel, bem como da existência de eventual avaria nele existente.</t>
   </si>
   <si>
     <t>5. Usei o serviço de “valet”existente em frente a um estabelecimento comercial – bar, restaurante, loja, teatro, casa noturna. Depois que retornei à minha residência, notei que meu veículo sofreu danos, mas não consigo entrar em contato com a empresa de “valet” para requerer o conserto. O que posso fazer?</t>
@@ -710,8 +673,7 @@
 d) Condições integrais da oferta, incluídas modalidades de pagamento, disponibilidade, forma e prazo da execução do serviço ou da entrega ou disponibilização do produto;
 e) Informações claras e ostensivas a respeito de quaisquer restrições à fruição da oferta;
 f) A quantidade mínima de consumidores para a efetivação do contrato;
-g) O prazo para utilização da oferta pelo consumidor.
-</t>
+g) O prazo para utilização da oferta pelo consumidor.</t>
   </si>
   <si>
     <t>5. Em quanto tempo as empresas devem responder às demandas de seus consumidores?</t>
@@ -728,8 +690,7 @@
   <si>
     <t>A compra e venda de veículo usado entre particulares, em regra, não é considerada uma relação de consumo, pois o vendedor, por não exercer a comercialização de veículos com habitualidade, não é considerado fornecedor pelo Código de Defesa do Consumidor.
 Por essa razão, essa espécie de contratação não está amparada pelo Código de Defesa do Consumidor. Nessa situação, são aplicáveis as regras do Código Civil.
-Apenas pessoas físicas que atuam com habitualidade na comercialização de veículos podem ser consideradas fornecedoras, de acordo com o artigo 3º do Código de Defesa do Consumidor. Nessa hipótese, a relação é de consumo, regida pelo Código de Defesa do Consumidor.
-</t>
+Apenas pessoas físicas que atuam com habitualidade na comercialização de veículos podem ser consideradas fornecedoras, de acordo com o artigo 3º do Código de Defesa do Consumidor. Nessa hipótese, a relação é de consumo, regida pelo Código de Defesa do Consumidor.</t>
   </si>
   <si>
     <t>2. Qual a documentação que devo exigir da revendedora/concessionária de veículos ao adquirir um carro usado?</t>
@@ -743,8 +704,7 @@
  - Contrato de venda.
 De acordo com a Lei nº 13.111/15, o contrato de venda deve conter cláusula contendo informações sobre:
  - a natureza e o valor dos tributos incidentes sobre a comercialização do veículo;
- - a situação de regularidade do veículo junto às autoridades policiais, fazendárias e de trânsito, inclusive eventuais registros e apontamentos que limitem ou impeçam a circulação do veículo.
-</t>
+ - a situação de regularidade do veículo junto às autoridades policiais, fazendárias e de trânsito, inclusive eventuais registros e apontamentos que limitem ou impeçam a circulação do veículo.</t>
   </si>
   <si>
     <t>3. Por que devo tomar mais cuidado ao comprar um carro usado? O que significa o termo “venda no estado”, geralmente inserida pela revendedora na nota fiscal ou recibo? Que cuidados devo tomar ao comprar um carro usado?</t>
@@ -752,8 +712,7 @@
   <si>
     <t>O consumidor deve tomar mais cuidado ao comprar um carro usado porque o vendedor não pode ser responsabilizado por vícios (problemas) ocultos decorrentes do desgaste natural causado pelo tempo e pela utilização do veículo. Esse entendimento vem sendo adotado de forma pacífica pelos Tribunais do país quando há discussão judicial a respeito.
 Nesse sentido, é bastante frequente que os revendedores de veículos usados insiram no recibo ou na nota fiscal a expressão “venda no estado”, que significa que o veículo não está em perfeitas condições. Nesse caso, peça ao fornecedor para descrever na nota fiscal ou recibo todos os problemas apresentados pelo veículo.
-Para evitar problemas no futuro, cumpre ao consumidor ser diligente e adotar alguns cuidados na hora de comprar um carro usado. O ideal é levar um mecânico de sua confiança para averiguar o estado do veículo antes de realizar a compra, principalmente o estado do motor, bombas e peças, bem como fazer uma vistoria cautelar do veículo com alguma empresa especializada.
-</t>
+Para evitar problemas no futuro, cumpre ao consumidor ser diligente e adotar alguns cuidados na hora de comprar um carro usado. O ideal é levar um mecânico de sua confiança para averiguar o estado do veículo antes de realizar a compra, principalmente o estado do motor, bombas e peças, bem como fazer uma vistoria cautelar do veículo com alguma empresa especializada.</t>
   </si>
   <si>
     <t>4. Há garantia na compra de um carro usado?</t>
@@ -763,8 +722,7 @@
 1) A troca do veículo por outro similar;
 2) O cancelamento da compra;
 3) O abatimento proporcional do preço (desconto).
-Para vícios (problemas) ocultos, isto é, de difícil constatação, o prazo para o consumidor reclamar também é de 90 dias, mas contados da data em que foi descoberto o vício.
-</t>
+Para vícios (problemas) ocultos, isto é, de difícil constatação, o prazo para o consumidor reclamar também é de 90 dias, mas contados da data em que foi descoberto o vício.</t>
   </si>
   <si>
     <t>5. A revendedora do veículo usado pode restringir a garantia ao motor e câmbio?</t>
@@ -773,8 +731,7 @@
     <t>O Código de Defesa do Consumidor prevê dois tipos de garantia, a legal e a contratual.
 A garantia legal, de observância obrigatória, é integral, ou seja, deve abranger todos os vícios (problemas) que o produto venha a apresentar. O fornecedor não pode limitá-la a determinados vícios. No caso dos veículos usados, a garantia legal é de 90 dias. Portanto, no caso de garantia legal, a revendedora de veículo não pode limitá-la ao câmbio e ao motor.
 A garantia contratual, também prevista no Código de Defesa do Consumidor, é complementar à garantia legal e pode ser parcial, isto é, limitar-se a determinados vícios (problemas). Portanto, no caso de veículos usados, a garantia contratual pode ser limitada apenas ao câmbio e ao motor.
-O prazo de garantia legal tem início após terminado o prazo da garantia contratual, quando existente.
-</t>
+O prazo de garantia legal tem início após terminado o prazo da garantia contratual, quando existente.</t>
   </si>
   <si>
     <t>Combustiveis</t>
@@ -805,8 +762,7 @@
 A adulteração dos combustíveis consiste na adição irregular de qualquer substância que modifique as suas características originais e a qualidade do produto, tornando-o inadequado ao uso. 
 A gasolina pode ser adulterada de várias formas. São frequentes a adição de álcool em quantidade superior à definida pela ANP e a mistura irregular de solventes.
 O álcool hidratado costuma ser adulterado por meio da adição de água. Também é frequente a adição de álcool anidro, que, de acordo com a ANP, pode ser adicionado tão somentetão somente à gasolina. Para evitar esse último tipo de fraude, a ANP, desde 2015, determina a adição de um corante alaranjado ao álcool anidro.
-O combustível adulterado pode trazer danos ao motor e a outros componentes dos automóveis, causar o rendimento insatisfatório do veículo, a perda de potência do motor e o aumento do consumo de combustível. A adulteração também causa danos ambientais, pois pode acarretar a elevação da contaminação por gases e partículas poluentes
-</t>
+O combustível adulterado pode trazer danos ao motor e a outros componentes dos automóveis, causar o rendimento insatisfatório do veículo, a perda de potência do motor e o aumento do consumo de combustível. A adulteração também causa danos ambientais, pois pode acarretar a elevação da contaminação por gases e partículas poluentes</t>
   </si>
   <si>
     <t>5. Como o consumidor pode saber se o combustível está adulterado?</t>
@@ -819,8 +775,7 @@
   </si>
   <si>
     <t>O consumidor que suspeite de adulteração deve denunciar o posto revendedor à Agência Nacional do Petróleo, Gás Natural e Biocombustíveis -ANP, na seção Fale Conosco do sítio eletrônico (http://www.anp.gov.br)  ou na Central de Atendimento 0800 970 0267 (ligação gratuita). Para o registro da denúncia é necessário informar o nome, o endereço, o CNPJ do estabelecimento e descrever o ocorrido.
-De acordo com a ANP, as denúncias recebidas, embora possam não resultar em imediata fiscalização, auxiliam a direcionar as ações e a estabelecer os roteiros da fiscalização.
-</t>
+De acordo com a ANP, as denúncias recebidas, embora possam não resultar em imediata fiscalização, auxiliam a direcionar as ações e a estabelecer os roteiros da fiscalização.</t>
   </si>
   <si>
     <t>7. Desconfio que houve diferença entre a quantidade de combustível que eu paguei e a que efetivamente foi colocada no tanque do meu veículo. O que devo fazer ?</t>
@@ -828,8 +783,7 @@
   <si>
     <t>Nesse caso, verifique se a bomba de combustíveis tem o selo obrigatório do Inmetro e peça ao posto para realizar o teste de vazão da bomba de combustível, no qual é utilizada a medida-padrão de 20 litros certificada pelo Inmetro. A diferença máxima permitida é de 100ml para mais ou para menos. 
 Se a diferença detectada for maior que 100 ml, denuncie o posto à ANP, na seção Fale Conosco do sítio eletrônico ( http://www.anp.gov.br)  ou na Central de Atendimento 0800 970 0267 (ligação gratuita). Para o registro da denúncia é necessário informar o nome, o endereço, o CNPJ do estabelecimento e a descrição do ocorrido.
-O posto é obrigado a realizar o teste quando solicitado pelo consumidor.
-</t>
+O posto é obrigado a realizar o teste quando solicitado pelo consumidor.</t>
   </si>
   <si>
     <t>8. Meu carro é flex (bicombustível). Quando é vantajoso abastecê-lo com álcool ?</t>
@@ -843,8 +797,7 @@
 CÁLCULO
 3,099 (preço da gasolina) X 0,7 = 2,1693 (resultado)
 ANÁLISE
-  2,1693 (resultado do cálculo) é menor que o preço do álcool (R$ 2,349). Logo, é vantajoso abastecer com gasolina.
-</t>
+  2,1693 (resultado do cálculo) é menor que o preço do álcool (R$ 2,349). Logo, é vantajoso abastecer com gasolina.</t>
   </si>
   <si>
     <t>Cobranca</t>
@@ -855,16 +808,14 @@
   <si>
     <t>Há a incidência de correção monetária, juros e multa.
 De acordo com o artigo 52 do Código de Defesa do Consumidor, as multas de mora não podem ser superiores a 2% (dois por cento) do valor da prestação.
-Caso não haja a previsão no contrato, incidirão juros de mora legais, de 1% ao mês, conforme estabelecem o artigo 406 do Código Civil e o artigo 161, §1º, do Código Tributário Nacional.
-</t>
+Caso não haja a previsão no contrato, incidirão juros de mora legais, de 1% ao mês, conforme estabelecem o artigo 406 do Código Civil e o artigo 161, §1º, do Código Tributário Nacional.</t>
   </si>
   <si>
     <t>2. Quais os meios de cobrança que podem ser empregados pelo fornecedor ?</t>
   </si>
   <si>
     <t>De acordo com o Código de Defesa do Consumidor, o fornecedor pode utilizar diferentes meios para efetuar cobrança, contudo não pode expor o consumidor a ridículo ou submetê-lo a qualquer tipo de constrangimento ou ameaça.
-Em todos os documentos de cobrança deverão constar o nome, o endereço e o número de inscrição no Cadastro de Pessoas Físicas – CPF ou no Cadastro Nacional de Pessoa Jurídica – CNPJ do fornecedor do produto ou serviço correspondente.
-</t>
+Em todos os documentos de cobrança deverão constar o nome, o endereço e o número de inscrição no Cadastro de Pessoas Físicas – CPF ou no Cadastro Nacional de Pessoa Jurídica – CNPJ do fornecedor do produto ou serviço correspondente.</t>
   </si>
   <si>
     <t>3. Tenho direito à devolução em dobro em caso de cobrança indevida?</t>
@@ -872,16 +823,14 @@
   <si>
     <t>O direito à devolução em dobro, previsto no artigo 42 do Código de Defesa do Consumidor, somente existe se o consumidor efetivamente pagou a conta cobrada indevidamente ou cobrada em valor excedente pelo fornecedor. Não basta que o consumidor seja cobrado a maior para ter direito a receber valor igual ao dobro.
 Não há direito à devolução em dobro se a cobrança indevida decorreu de erro justificável por parte do fornecedor.
-Apesar de não constar esse requisito no Código de Defesa do Consumidor, o Superior Tribunal de Justiça (STJ), ao se manifestar sobre a questão, consolidou entendimento de que o consumidor só tem direito à restituição em dobro caso seja comprovada má-fé do fornecedor ao realizar a cobrança.
-</t>
+Apesar de não constar esse requisito no Código de Defesa do Consumidor, o Superior Tribunal de Justiça (STJ), ao se manifestar sobre a questão, consolidou entendimento de que o consumidor só tem direito à restituição em dobro caso seja comprovada má-fé do fornecedor ao realizar a cobrança.</t>
   </si>
   <si>
     <t>4. É legal a cobrança decorrente de renovação automática de assinaturas de produtos ou serviços ?</t>
   </si>
   <si>
     <t>É frequente que os fornecedores disponibilizem gratuitamente determinado serviço, por certo período, e passem a cobrar por ele se o consumidor não solicitar o cancelamento até o escoamento do prazo de gratuidade.
-No entanto, de acordo com o Código de Defesa do Consumidor, é abusiva a renovação automática de assinaturas de produtos e serviços. Desse modo, a consequente cobrança é ilegal. O consumidor deve sempre concordar expressamente com a renovação da assinatura de produtos ou serviços.
-</t>
+No entanto, de acordo com o Código de Defesa do Consumidor, é abusiva a renovação automática de assinaturas de produtos e serviços. Desse modo, a consequente cobrança é ilegal. O consumidor deve sempre concordar expressamente com a renovação da assinatura de produtos ou serviços.</t>
   </si>
   <si>
     <t>5. É legal a cobrança de taxa pela emissão de boletos ?</t>
@@ -901,15 +850,13 @@
 • 1 ano para as dívidas com hospedagem e alimentação, bem como com seguradoras;
 • 3 anos para as dívidas referentes a aluguéis e para as dívidas de juros em que o principal já foi pago;
 • 5 anos para as demais dívidas e cheques devolvidos por falta de fundos que foram registrados no Cadastro de Emitentes de Cheques sem Fundos (CCF).
- Os prazos acima são contados da data da em que o consumidor se tornou inadimplente e não da data em que o nome do consumidor foi inserido no cadastro de proteção ao crédito.
-</t>
+ Os prazos acima são contados da data da em que o consumidor se tornou inadimplente e não da data em que o nome do consumidor foi inserido no cadastro de proteção ao crédito.</t>
   </si>
   <si>
     <t>2. O nome do consumidor pode ser inserido nos cadastros de proteção ao crédito – SPC, SERASA, CCF – sem que haja prévia notificação ?</t>
   </si>
   <si>
-    <t>Não. O consumidor deve ser sempre notificado  a respeito pelo órgão mantenedor do cadastro de proteção ao crédito, antes da inclusão de seu nome no banco de dados.
-</t>
+    <t>Não. O consumidor deve ser sempre notificado  a respeito pelo órgão mantenedor do cadastro de proteção ao crédito, antes da inclusão de seu nome no banco de dados.</t>
   </si>
   <si>
     <t>3. Sempre há direito a indenização por danos morais quando o nome do consumidor é inserido indevidamente nos cadastros de proteção ao crédito ?</t>
@@ -930,8 +877,7 @@
     <t>O “score” de crédito é um método estatístico de avaliação de risco de inadimplência  que emprega dados públicos ( informações do censo, índice de inadimplência por região, pesquisas sobre o mercado de trabalho, etc.), informações legalmente fornecidas pelo próprio consumidor e dados relativos ao comportamento do consumidor em relação ao crédito (registros de débitos inadimplidos apontados por empresas credoras, quantidade de consultas realizadas, valores dos débitos, diversidade de segmentos em que os débitos foram registrados, existência ou não de ação judicial e títulos protestados).
 O “score” de crédito pode ser empregado pelos fornecedores para negar crédito ao consumidor.
 O Superior Tribunal de Justiça já decidiu que o “score” de crédito não constitui banco de dados, dispensa o consentimento do consumidor e pode ser utilizado como método de avaliação do risco de inadimplência.
-Não obstante, o consumidor possui o direito de solicitar esclarecimentos sobre as informações pessoais valoradas e as fontes dos dados consideradas no respectivo cálculo do “score”.
-</t>
+Não obstante, o consumidor possui o direito de solicitar esclarecimentos sobre as informações pessoais valoradas e as fontes dos dados consideradas no respectivo cálculo do “score”.</t>
   </si>
   <si>
     <t>Cadastros positivos de crédito</t>
@@ -941,15 +887,14 @@
   </si>
   <si>
     <t>Os cadastros positivos de crédito, disciplinados pela Lei nº 12.414/11, são bancos de dados com informações de adimplemento de dívidas e de cumprimento de outras obrigações pecuniárias por pessoas naturais ou pessoas jurídicas, para formação de um histórico de crédito.
-Esses cadastros visam subsidiar a concessão de crédito, a realização de venda a prazo ou de outras transações comerciais e empresariais que impliquem risco financeiro aos fornecedores. Surgiram também com a proposta de possibilitar a oferta de crédito em condições mais vantajosas para o consumidor.
-</t>
-  </si>
-  <si>
-    <t>2. É vantajoso ao consumidor participar do cadastro positivo de crédito? </t>
+Esses cadastros visam subsidiar a concessão de crédito, a realização de venda a prazo ou de outras transações comerciais e empresariais que impliquem risco financeiro aos fornecedores. Surgiram também com a proposta de possibilitar a oferta de crédito em condições mais vantajosas para o consumidor.</t>
+  </si>
+  <si>
+    <t>2. É vantajoso ao consumidor participar do cadastro positivo de crédito?</t>
   </si>
   <si>
     <r>
-      <t>(COMENTÁRIO: </t>
+      <t>(COMENTÁRIO:</t>
     </r>
     <r>
       <rPr>
@@ -968,12 +913,11 @@
         <charset val="1"/>
       </rPr>
       <t>o.)                                              Na prática, o cadastro positivo não tem se revelado útil aos consumidores porque sua principal vantagem, que seria propiciar a oferta de crédito em condições mais vantajosas aos bons pagadores, não vem sendo assegurada por nenhuma das instituições financeiras gestoras desses cadastros.
-Até o momento, infelizmente, o cadastro positivo é uma via de mão única, pois permite apenas o fornecimento dos dados dos consumidores aos gestores desses cadastros, porém os consumidores, na prática, não têm sido beneficiados.
-</t>
+Até o momento, infelizmente, o cadastro positivo é uma via de mão única, pois permite apenas o fornecimento dos dados dos consumidores aos gestores desses cadastros, porém os consumidores, na prática, não têm sido beneficiados.</t>
     </r>
   </si>
   <si>
-    <t>3. O consumidor pode ser incluído no cadastro positivo sem o seu consentimento? </t>
+    <t>3. O consumidor pode ser incluído no cadastro positivo sem o seu consentimento?</t>
   </si>
   <si>
     <t>Não. A participação do consumidor no cadastro positivo depende de sua autorização prévia, mediante consentimento informado por meio de assinatura em instrumento específico ou cláusula apartada para esse fim.</t>
@@ -982,13 +926,13 @@
     <t>4. O consumidor pode requerer o cancelamento da autorização de inclusão de suas informações no cadastro positivo?</t>
   </si>
   <si>
-    <t>Sim. De acordo com o artigo 5º da Lei nº 12.414/11, o consumidor possui o direito de obter o cancelamento de seu cadastro, quando solicitado. </t>
+    <t>Sim. De acordo com o artigo 5º da Lei nº 12.414/11, o consumidor possui o direito de obter o cancelamento de seu cadastro, quando solicitado.</t>
   </si>
   <si>
     <t>5. Como se dá a responsabilidade pelos danos causados ao consumidor participante dos cadastros positivos?</t>
   </si>
   <si>
-    <t>O gestor do cadastro positivo, as pessoas jurídicas que atuaram como fontes para o cadastro e os consulentes do cadastro são responsáveis objetiva e solidariamente pelos danos materiais e morais causados ao consumidor. </t>
+    <t>O gestor do cadastro positivo, as pessoas jurídicas que atuaram como fontes para o cadastro e os consulentes do cadastro são responsáveis objetiva e solidariamente pelos danos materiais e morais causados ao consumidor.</t>
   </si>
   <si>
     <t>6. Por quanto tempo as informações de adimplemento poderão constar do cadastro positivo?</t>
@@ -1005,8 +949,7 @@
   <si>
     <t>A taxa de serviço, geralmente cobrada pelos restaurantes no valor de 10% do total consumido, corresponde à gorjeta dos funcionários (garçons). O consumidor não é obrigado a pagá-la, pois a remuneração dos funcionários do restaurante é de responsabilidade de seu proprietário. 
 Os estabelecimentos devem informar previamente ao consumidor que cobram a taxa de serviço, apontar qual o percentual que utilizam para calculá-la e esclarecer que o seu pagamento é facultativo.
-A cobrança obrigatória da taxa de serviço constitui prática abusiva.
-</t>
+A cobrança obrigatória da taxa de serviço constitui prática abusiva.</t>
   </si>
   <si>
     <t>2. O pagamento do “couvert” servido nos restaurantes é obrigatório ?</t>
@@ -1014,8 +957,7 @@
   <si>
     <t>O “couvert” é o serviço caracterizado pelo fornecimento de aperitivos/petiscos antes do início da refeição propriamente dita.
 De acordo com a Lei Estadual nº 14.536/11, é proibido o fornecimento do serviço de “couvert” ao consumidor sem solicitação prévia, salvo se foi oferecido pelo estabelecimento gratuitamente.
-Se o consumidor não solicitou o “couvert” e o mesmo foi fornecido pelo estabelecimento, sem qualquer aviso prévio de sua cobrança, o consumidor não deve pagá-lo.
-</t>
+Se o consumidor não solicitou o “couvert” e o mesmo foi fornecido pelo estabelecimento, sem qualquer aviso prévio de sua cobrança, o consumidor não deve pagá-lo.</t>
   </si>
   <si>
     <t>3. O que é “couvert” artístico ? Seu pagamento é obrigatório ?</t>
@@ -1023,16 +965,14 @@
   <si>
     <t>“Couvert” artístico é uma taxa cobrada por bares e casas noturnas pela música ao vivo ou música eletrônica colocadas à disposição dos frequentadores.
 O seu pagamento é obrigatório, porém, de acordo com a Lei Estadual nº 12.278/06, os estabelecimentos que exploram música ou vivo ou música eletrônica são obrigados a informar previamente o valor da taxa de “couvert” artístico ao consumidor, por meio de placas informativas.
-Caso o consumidor não seja informado previamente sobre a taxa de “couvert” artístico, sua cobrança é indevida.
-</t>
+Caso o consumidor não seja informado previamente sobre a taxa de “couvert” artístico, sua cobrança é indevida.</t>
   </si>
   <si>
     <t>4. Os bares e casas noturnas podem cobrar consumação mínima ?</t>
   </si>
   <si>
     <t>Não. A consumação mínima, além de configurar venda casada (pagamento pela entrada e fornecimento de alimentos e/ou bebidas), implica na imposição de limites quantitativos de consumo, práticas consideradas abusivas pelo artigo 
-39 do Código de Defesa do Consumidor.
-</t>
+39 do Código de Defesa do Consumidor.</t>
   </si>
   <si>
     <t>5. Perdi a comanda que controlava meu consumo no bar ou casa noturna. Sou obrigado a pagar taxa pela perda ?</t>
@@ -1050,10 +990,10 @@
     <t>Produtos</t>
   </si>
   <si>
-    <t>1.9. O que é produto? </t>
-  </si>
-  <si>
-    <t>Segundo o art. 3º, da Lei federal nº 8.078/90, produto é qualquer bem, móvel ou imóvel, material ou imaterial. </t>
+    <t>1.9. O que é produto?</t>
+  </si>
+  <si>
+    <t>Segundo o art. 3º, da Lei federal nº 8.078/90, produto é qualquer bem, móvel ou imóvel, material ou imaterial.</t>
   </si>
   <si>
     <t>Produtos viciados</t>
@@ -1069,20 +1009,19 @@
 III - os produtos que, por qualquer motivo, se revelem inadequados ao fim a que se destinam.
 b) se, consideradas a qualidade e a quantidade, for inadequado para o consumo.
 c) vícios de qualidade ou quantidade que diminuam o valor do produto.
-Frise-se que, conforme o Código de Defesa do Consumidor, vícios de quantidade são aqueles que respeitadas as variações decorrentes de sua natureza, seu conteúdo líquido for inferior às indicações constantes do recipiente, da embalagem, rotulagem ou de mensagem publicitária.
-</t>
+Frise-se que, conforme o Código de Defesa do Consumidor, vícios de quantidade são aqueles que respeitadas as variações decorrentes de sua natureza, seu conteúdo líquido for inferior às indicações constantes do recipiente, da embalagem, rotulagem ou de mensagem publicitária.</t>
   </si>
   <si>
     <t>2.2. Qual o prazo legal para a substituição das partes viciadas? O consumidor e o fornecedor podem combinar outros prazos?</t>
   </si>
   <si>
-    <t>O prazo é de 30 dias, salvo se as partes (consumidor e fornecedor) não contratarem prazo diverso, não podendo este ser inferior a 7 dias ou superior a 180 dias. </t>
+    <t>O prazo é de 30 dias, salvo se as partes (consumidor e fornecedor) não contratarem prazo diverso, não podendo este ser inferior a 7 dias ou superior a 180 dias.</t>
   </si>
   <si>
     <t>2.3. Quais são as providências que o consumidor pode adotar se os vícios não forem sanados no prazo legal ou no prazo combinado?</t>
   </si>
   <si>
-    <t>O consumidor poderá exigir a) a substituição do produto por outro da mesma espécie, em perfeitas condições de uso;b) a restituição imediata da quantia paga, monetariamente atualizada, sem prejuízo de eventuais perdas e danos; ou c) o abatimento proporcional do preço.Além de uma dessas exigências, se a situação envolver vício de quantidade, o consumidor poderá exigir acomplementação do peso ou medida. </t>
+    <t>O consumidor poderá exigir a) a substituição do produto por outro da mesma espécie, em perfeitas condições de uso;b) a restituição imediata da quantia paga, monetariamente atualizada, sem prejuízo de eventuais perdas e danos; ou c) o abatimento proporcional do preço.Além de uma dessas exigências, se a situação envolver vício de quantidade, o consumidor poderá exigir acomplementação do peso ou medida.</t>
   </si>
   <si>
     <t>2.4. Mas e se os prazos estabelecidos na lei ou no contrato inviabilizarem o produto, seu consumo ou seu uso?</t>
@@ -1113,8 +1052,7 @@
   </si>
   <si>
     <t>Contrato de adesão é aquele cujas cláusulas tenham sido aprovadas pela autoridade competente ou estabelecidas unilateralmente pelo fornecedor de produtos ou serviços, sem que o consumidor possa discutir ou modificar substancialmente seu conteúdo.  Assim, o consumidor apenas adere ao contrato sem ter o poder de alterar suas cláusulas. 
-O Código de Defesa do Consumidor prevê que as cláusulas de alteração de prazo (devem ser convencionadas em separado, por meio de manifestação expressa do consumidor.
-</t>
+O Código de Defesa do Consumidor prevê que as cláusulas de alteração de prazo (devem ser convencionadas em separado, por meio de manifestação expressa do consumidor.</t>
   </si>
   <si>
     <t>Servicos</t>
@@ -1126,7 +1064,7 @@
     <t>Segundo o art. 3º, da Lei federal nº 8.078/90, serviço é qualquer atividade fornecida no mercado de consumo, mediante remuneração, inclusive as de natureza bancária, financeira, de crédito e securitária, salvo as decorrentes das relações de caráter trabalhista.”</t>
   </si>
   <si>
-    <t>Sevicos Publicos </t>
+    <t>Sevicos Publicos</t>
   </si>
   <si>
     <t>2.11. O serviços públicos são serviços para fins do direito do consumidor ?</t>
@@ -1168,24 +1106,21 @@
     <t>O consumidor poderá exigir:
 a) a reexecução dos serviços, sem custo adicional e quando cabível;
 b) a restituição imediata da quantia paga, monetariamente atualizada, sem prejuízo de eventuais perdas e danos; ou
-c)o abatimento proporcional do preço.
-</t>
+c)o abatimento proporcional do preço.</t>
   </si>
   <si>
     <t>2.9. O consumidor poderá contratar terceiro para resolver o vício do serviço?</t>
   </si>
   <si>
     <t>Sim, desde que o fornecedor se negue a resolver o vício ou não responda sobre o problema em prazo razoável..
-Além disso, o fornecedor poderá indicar terceiro devidamente capacitado para realizar o serviço, desde que não constitua uma obrigação personalíssima, ou seja,desde que não se trate de serviço que apenas pode ser realizado pessoalmente pelo fornecedor.
-</t>
+Além disso, o fornecedor poderá indicar terceiro devidamente capacitado para realizar o serviço, desde que não constitua uma obrigação personalíssima, ou seja,desde que não se trate de serviço que apenas pode ser realizado pessoalmente pelo fornecedor.</t>
   </si>
   <si>
     <t>2.10. Se o serviço tiver como objetivo a reparação de produtos, quais as peças deverão ser utilizadas se necessária a substituição da peça?</t>
   </si>
   <si>
     <t>No fornecimento de serviços que tenham por objetivo a reparação de qualquer produto considerar-se-á implícita a obrigação do fornecedor de empregar componentes de reposição originais adequados e novos, ou que mantenham as especificações técnicas do fabricante, salvo, quanto a estes últimos, autorização em contrário do consumidor.
-Em outras palavras, mesmo que não se encontre explícita no contrato, muitas vezes verbal (não escrito), há obrigação do fornecedor em substituir peças quebradas, defeituosas, estragadas, por peças originais e/ou, no máximo, peças que tenhas as mesmas especificações técnicas determinadas pelos fabricantes dos produtos.
-</t>
+Em outras palavras, mesmo que não se encontre explícita no contrato, muitas vezes verbal (não escrito), há obrigação do fornecedor em substituir peças quebradas, defeituosas, estragadas, por peças originais e/ou, no máximo, peças que tenhas as mesmas especificações técnicas determinadas pelos fabricantes dos produtos.</t>
   </si>
   <si>
     <t>Legislacao</t>
@@ -1201,8 +1136,7 @@
 Essa legislação foi regulamentada pelos seguintes Decretos federais:
 Decreto nº 2.181/97 -dispõe sobre a organização do Sistema Nacional de Defesa do Consumidor – SNDC e estabelece as normas gerais de aplicação das sanções administrativas previstas na Lei nº 8.078, de 11 de setembro de 1990
 Decreto nº 5.903/06 – fixa regras sobre informação adequada sobre produtos e serviços;
-Decreto nº 6.523/08 - fixa normas gerais sobre o Serviço de Atendimento ao Consumidor – SAC;
-</t>
+Decreto nº 6.523/08 - fixa normas gerais sobre o Serviço de Atendimento ao Consumidor – SAC;</t>
   </si>
   <si>
     <t>TIRE SUAS DUVIDAS</t>
@@ -1219,8 +1153,7 @@
   <si>
     <t>Segundo o Código de Defesa do Consumidor, (Art. 2°) consumidor é toda pessoa física ou jurídica que adquire ou utiliza produto ou serviço como destinatário final.
 Ser destinatário final significa ser consumidor não profissional, ou seja, adquirir ou utilizar o produto para uso próprio ou familiar.
-Excepcionalmente, outras pessoas podem ser consideradas consumidoras quando, no caso concreto, manifestarem vulnerabilidade na relação de consumo.
-</t>
+Excepcionalmente, outras pessoas podem ser consideradas consumidoras quando, no caso concreto, manifestarem vulnerabilidade na relação de consumo.</t>
   </si>
   <si>
     <t>1.3. Mesmo que eu não compre o bem ou o serviço, posso ser considerado consumidor?</t>
@@ -1239,8 +1172,7 @@
   </si>
   <si>
     <t>Sim. Para isso, basta que elas adquiram ou utilizem o bem ou serviço para satisfazer suas necessidades, ou seja, como destinatárias finais, ou, ainda, demonstrem vulnerabilidade técnica, econômica ou jurídica no caso concreto.
-Exemplo: a aquisição de cadeiras ou bancos para uso de seus associados/funcionários.
-</t>
+Exemplo: a aquisição de cadeiras ou bancos para uso de seus associados/funcionários.</t>
   </si>
   <si>
     <t>1.6. Um grupo de pessoas pode ser considerado consumidor? Ou apenas pessoas (físicas ou jurídicas) podem ser consideradas consumidoras?</t>
@@ -1271,8 +1203,7 @@
   </si>
   <si>
     <r>
-      <t>Caso o defeito seja do PRODUTO:
-</t>
+      <t>Caso o defeito seja do PRODUTO:</t>
     </r>
     <r>
       <rPr>
@@ -1282,14 +1213,12 @@
         <charset val="1"/>
       </rPr>
       <t>a) O fabricante, o produtor, o construtor, nacional ou estrangeiro, e o importador respondem,independentemente da existência de culpa, pela reparação dos danos causados aos consumidores por defeitos decorrentes de projeto, fabricação, construção, montagem, fórmulas, manipulação, apresentação ou acondicionamento de seus produtos, bem como por informações insuficientes ou inadequadas sobre sua utilização e riscos;
-b) O comerciante é igualmente responsável, quandoo fabricante, o construtor, o produtor ou o importador não puderem ser identificados;quando o produto for fornecido sem identificação clara do seu fabricante, produtor, construtor ou importador; ou, ainda, senão conservar adequadamente os produtos perecíveis.
-</t>
+b) O comerciante é igualmente responsável, quandoo fabricante, o construtor, o produtor ou o importador não puderem ser identificados;quando o produto for fornecido sem identificação clara do seu fabricante, produtor, construtor ou importador; ou, ainda, senão conservar adequadamente os produtos perecíveis.</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Caso o defeito seja do SERVIÇO:
-</t>
+      <t>Caso o defeito seja do SERVIÇO:</t>
     </r>
     <r>
       <rPr>
@@ -1298,8 +1227,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>a)Todos os fornecedores de serviços, inclusive o comerciante,respondem, independentemente da existência de culpa, pela reparação dos danos causados aos consumidores por defeitos relativos à prestação dos serviços, bem como por informações insuficientes ou inadequadas sobre sua fruição e riscos.
-</t>
+      <t>a)Todos os fornecedores de serviços, inclusive o comerciante,respondem, independentemente da existência de culpa, pela reparação dos danos causados aos consumidores por defeitos relativos à prestação dos serviços, bem como por informações insuficientes ou inadequadas sobre sua fruição e riscos.</t>
     </r>
   </si>
   <si>
@@ -1313,8 +1241,7 @@
   </si>
   <si>
     <t>O que se espera das relações de consumo é que as partes entrem em entendimento e respeitem-se mutuamente, reconhecendo os problemas e resolvendo-os.
-No entanto, se o consumidor não conseguir ser atendido em seu pleito, poderá recorrer aos órgãos administrativos existentes (como por ex. o PROCON Paulistano) ou ao Poder Judiciário, por intermédio de ação judicial.
-</t>
+No entanto, se o consumidor não conseguir ser atendido em seu pleito, poderá recorrer aos órgãos administrativos existentes (como por ex. o PROCON Paulistano) ou ao Poder Judiciário, por intermédio de ação judicial.</t>
   </si>
   <si>
     <t>PRISCILLA</t>
@@ -2127,8 +2054,8 @@
   </sheetPr>
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A148" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A160" activeCellId="0" sqref="A160"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A147" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A151" activeCellId="0" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25"/>
@@ -2411,7 +2338,7 @@
       <c r="B25" s="19"/>
       <c r="C25" s="28"/>
     </row>
-    <row r="26" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="29" t="s">
         <v>54</v>
       </c>
@@ -2422,8 +2349,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="29"/>
+    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="B27" s="30" t="s">
         <v>57</v>
       </c>
@@ -2431,8 +2360,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="29"/>
+    <row r="28" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="B28" s="30" t="s">
         <v>59</v>
       </c>
@@ -2440,8 +2371,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="29"/>
+    <row r="29" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="B29" s="30" t="s">
         <v>61</v>
       </c>
@@ -2449,8 +2382,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="29"/>
+    <row r="30" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="B30" s="30" t="s">
         <v>63</v>
       </c>
@@ -2587,7 +2522,9 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="146.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="38"/>
+      <c r="A43" s="38" t="s">
+        <v>87</v>
+      </c>
       <c r="B43" s="39" t="s">
         <v>90</v>
       </c>
@@ -2596,7 +2533,9 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="409.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="38"/>
+      <c r="A44" s="38" t="s">
+        <v>87</v>
+      </c>
       <c r="B44" s="39" t="s">
         <v>92</v>
       </c>
@@ -2605,21 +2544,27 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="375.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="38"/>
+      <c r="A45" s="38" t="s">
+        <v>87</v>
+      </c>
       <c r="B45" s="39"/>
       <c r="C45" s="42" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="204.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="38"/>
+      <c r="A46" s="38" t="s">
+        <v>87</v>
+      </c>
       <c r="B46" s="39"/>
       <c r="C46" s="43" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="268.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="38"/>
+      <c r="A47" s="38" t="s">
+        <v>87</v>
+      </c>
       <c r="B47" s="44" t="s">
         <v>96</v>
       </c>
@@ -2627,8 +2572,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="220.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="38"/>
+    <row r="48" customFormat="false" ht="156.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="38" t="s">
+        <v>87</v>
+      </c>
       <c r="B48" s="44" t="s">
         <v>98</v>
       </c>
@@ -2647,8 +2594,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="45"/>
+    <row r="50" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="45" t="s">
+        <v>100</v>
+      </c>
       <c r="B50" s="46" t="s">
         <v>103</v>
       </c>
@@ -2657,7 +2606,9 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="160.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="45"/>
+      <c r="A51" s="45" t="s">
+        <v>100</v>
+      </c>
       <c r="B51" s="46" t="s">
         <v>105</v>
       </c>
@@ -2665,8 +2616,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="45"/>
+    <row r="52" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="45" t="s">
+        <v>100</v>
+      </c>
       <c r="B52" s="46" t="s">
         <v>107</v>
       </c>
@@ -2675,7 +2628,9 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="175.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="45"/>
+      <c r="A53" s="45" t="s">
+        <v>100</v>
+      </c>
       <c r="B53" s="9" t="s">
         <v>109</v>
       </c>
@@ -3800,11 +3755,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A42:A48"/>
+  <mergeCells count="2">
     <mergeCell ref="B44:B46"/>
-    <mergeCell ref="A49:A53"/>
     <mergeCell ref="B148:B149"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>